<commit_message>
Added code for scrapping MRM
</commit_message>
<xml_diff>
--- a/processed/jmri-all-summary.xlsx
+++ b/processed/jmri-all-summary.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukaizou/Google Drive/UHS-MRIPhysics-journal-web-scrapping/processed/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00354343-D682-B84F-895D-10775D264288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jmri-vol-54-no-1" sheetId="1" r:id="rId1"/>
     <sheet name="jmri-vol-54-no-2" sheetId="2" r:id="rId2"/>
     <sheet name="jmri-vol-54-no-3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1179,8 +1185,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1256,6 +1262,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1302,7 +1316,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1334,9 +1348,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1368,6 +1400,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1543,14 +1593,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="213.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1584,7 +1643,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1601,7 +1660,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1618,7 +1677,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1635,7 +1694,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1652,7 +1711,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1669,7 +1728,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1686,7 +1745,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1762,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1720,7 +1779,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1737,7 +1796,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1813,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1771,7 +1830,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1788,7 +1847,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1805,7 +1864,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1822,7 +1881,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1839,7 +1898,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1856,7 +1915,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1873,7 +1932,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1949,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1907,7 +1966,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1924,7 +1983,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1941,7 +2000,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1958,7 +2017,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -1975,7 +2034,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -1992,7 +2051,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -2009,7 +2068,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -2026,7 +2085,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -2043,7 +2102,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -2060,7 +2119,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2077,7 +2136,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2094,7 +2153,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2111,7 +2170,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2187,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2145,7 +2204,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2162,7 +2221,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2179,7 +2238,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2196,7 +2255,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2213,7 +2272,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -2230,7 +2289,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2247,7 +2306,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2264,7 +2323,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2281,7 +2340,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2298,7 +2357,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -2317,64 +2376,73 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E31" r:id="rId30"/>
-    <hyperlink ref="E32" r:id="rId31"/>
-    <hyperlink ref="E33" r:id="rId32"/>
-    <hyperlink ref="E34" r:id="rId33"/>
-    <hyperlink ref="E35" r:id="rId34"/>
-    <hyperlink ref="E36" r:id="rId35"/>
-    <hyperlink ref="E37" r:id="rId36"/>
-    <hyperlink ref="E38" r:id="rId37"/>
-    <hyperlink ref="E39" r:id="rId38"/>
-    <hyperlink ref="E40" r:id="rId39"/>
-    <hyperlink ref="E41" r:id="rId40"/>
-    <hyperlink ref="E42" r:id="rId41"/>
-    <hyperlink ref="E43" r:id="rId42"/>
-    <hyperlink ref="E44" r:id="rId43"/>
-    <hyperlink ref="E45" r:id="rId44"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="157.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -2408,7 +2476,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -2425,7 +2493,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -2442,7 +2510,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -2459,7 +2527,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -2476,7 +2544,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>139</v>
       </c>
@@ -2493,7 +2561,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>139</v>
       </c>
@@ -2510,7 +2578,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>139</v>
       </c>
@@ -2527,7 +2595,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>139</v>
       </c>
@@ -2544,7 +2612,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -2561,7 +2629,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>139</v>
       </c>
@@ -2578,7 +2646,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -2595,7 +2663,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -2612,7 +2680,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -2629,7 +2697,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -2646,7 +2714,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -2663,7 +2731,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -2680,7 +2748,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>139</v>
       </c>
@@ -2697,7 +2765,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>139</v>
       </c>
@@ -2714,7 +2782,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -2731,7 +2799,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>139</v>
       </c>
@@ -2748,7 +2816,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>139</v>
       </c>
@@ -2765,7 +2833,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -2782,7 +2850,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>139</v>
       </c>
@@ -2799,7 +2867,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -2816,7 +2884,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -2833,7 +2901,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -2850,7 +2918,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>139</v>
       </c>
@@ -2867,7 +2935,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -2884,7 +2952,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>139</v>
       </c>
@@ -2901,7 +2969,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>139</v>
       </c>
@@ -2918,7 +2986,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -2935,7 +3003,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -2952,7 +3020,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -2969,7 +3037,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -2986,7 +3054,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -3003,7 +3071,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>139</v>
       </c>
@@ -3020,7 +3088,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>139</v>
       </c>
@@ -3037,7 +3105,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -3054,7 +3122,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>139</v>
       </c>
@@ -3071,7 +3139,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>139</v>
       </c>
@@ -3088,7 +3156,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3105,7 +3173,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>139</v>
       </c>
@@ -3122,7 +3190,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>139</v>
       </c>
@@ -3141,64 +3209,73 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E31" r:id="rId30"/>
-    <hyperlink ref="E32" r:id="rId31"/>
-    <hyperlink ref="E33" r:id="rId32"/>
-    <hyperlink ref="E34" r:id="rId33"/>
-    <hyperlink ref="E35" r:id="rId34"/>
-    <hyperlink ref="E36" r:id="rId35"/>
-    <hyperlink ref="E37" r:id="rId36"/>
-    <hyperlink ref="E38" r:id="rId37"/>
-    <hyperlink ref="E39" r:id="rId38"/>
-    <hyperlink ref="E40" r:id="rId39"/>
-    <hyperlink ref="E41" r:id="rId40"/>
-    <hyperlink ref="E42" r:id="rId41"/>
-    <hyperlink ref="E43" r:id="rId42"/>
-    <hyperlink ref="E44" r:id="rId43"/>
-    <hyperlink ref="E45" r:id="rId44"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="E31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="E36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="E37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="E39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="E40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="E42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="E43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="E44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="E45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="180.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3215,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>254</v>
       </c>
@@ -3232,7 +3309,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>254</v>
       </c>
@@ -3249,7 +3326,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>254</v>
       </c>
@@ -3266,7 +3343,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -3283,7 +3360,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>254</v>
       </c>
@@ -3300,7 +3377,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>254</v>
       </c>
@@ -3317,7 +3394,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>254</v>
       </c>
@@ -3334,7 +3411,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>254</v>
       </c>
@@ -3351,7 +3428,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -3368,7 +3445,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>254</v>
       </c>
@@ -3385,7 +3462,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -3402,7 +3479,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>254</v>
       </c>
@@ -3419,7 +3496,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>254</v>
       </c>
@@ -3436,7 +3513,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>254</v>
       </c>
@@ -3453,7 +3530,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>254</v>
       </c>
@@ -3470,7 +3547,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>254</v>
       </c>
@@ -3487,7 +3564,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>254</v>
       </c>
@@ -3504,7 +3581,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>254</v>
       </c>
@@ -3521,7 +3598,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>254</v>
       </c>
@@ -3538,7 +3615,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>254</v>
       </c>
@@ -3555,7 +3632,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>254</v>
       </c>
@@ -3572,7 +3649,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -3589,7 +3666,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>254</v>
       </c>
@@ -3606,7 +3683,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>254</v>
       </c>
@@ -3623,7 +3700,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>254</v>
       </c>
@@ -3640,7 +3717,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>254</v>
       </c>
@@ -3657,7 +3734,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>254</v>
       </c>
@@ -3674,7 +3751,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>254</v>
       </c>
@@ -3691,7 +3768,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>254</v>
       </c>
@@ -3708,7 +3785,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>254</v>
       </c>
@@ -3725,7 +3802,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>254</v>
       </c>
@@ -3742,7 +3819,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>254</v>
       </c>
@@ -3759,7 +3836,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>254</v>
       </c>
@@ -3776,7 +3853,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>254</v>
       </c>
@@ -3793,7 +3870,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>254</v>
       </c>
@@ -3810,7 +3887,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>254</v>
       </c>
@@ -3827,7 +3904,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>254</v>
       </c>
@@ -3844,7 +3921,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>254</v>
       </c>
@@ -3861,7 +3938,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>254</v>
       </c>
@@ -3878,7 +3955,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>254</v>
       </c>
@@ -3895,7 +3972,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>254</v>
       </c>
@@ -3912,7 +3989,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>254</v>
       </c>
@@ -3929,7 +4006,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>254</v>
       </c>
@@ -3946,7 +4023,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>254</v>
       </c>
@@ -3963,7 +4040,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>254</v>
       </c>
@@ -3980,7 +4057,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>254</v>
       </c>
@@ -3997,7 +4074,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>254</v>
       </c>
@@ -4014,7 +4091,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>254</v>
       </c>
@@ -4031,7 +4108,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>254</v>
       </c>
@@ -4048,7 +4125,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>254</v>
       </c>
@@ -4065,7 +4142,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>254</v>
       </c>
@@ -4084,57 +4161,57 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
-    <hyperlink ref="E30" r:id="rId29"/>
-    <hyperlink ref="E31" r:id="rId30"/>
-    <hyperlink ref="E32" r:id="rId31"/>
-    <hyperlink ref="E33" r:id="rId32"/>
-    <hyperlink ref="E34" r:id="rId33"/>
-    <hyperlink ref="E35" r:id="rId34"/>
-    <hyperlink ref="E36" r:id="rId35"/>
-    <hyperlink ref="E37" r:id="rId36"/>
-    <hyperlink ref="E38" r:id="rId37"/>
-    <hyperlink ref="E39" r:id="rId38"/>
-    <hyperlink ref="E40" r:id="rId39"/>
-    <hyperlink ref="E41" r:id="rId40"/>
-    <hyperlink ref="E42" r:id="rId41"/>
-    <hyperlink ref="E43" r:id="rId42"/>
-    <hyperlink ref="E44" r:id="rId43"/>
-    <hyperlink ref="E45" r:id="rId44"/>
-    <hyperlink ref="E46" r:id="rId45"/>
-    <hyperlink ref="E47" r:id="rId46"/>
-    <hyperlink ref="E48" r:id="rId47"/>
-    <hyperlink ref="E49" r:id="rId48"/>
-    <hyperlink ref="E50" r:id="rId49"/>
-    <hyperlink ref="E51" r:id="rId50"/>
-    <hyperlink ref="E52" r:id="rId51"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="E31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="E36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="E37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="E39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="E40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="E42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="E43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="E44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="E45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="E46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="E47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="E48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="E49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="E50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="E51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="E52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>